<commit_message>
team profile edit halfway done
</commit_message>
<xml_diff>
--- a/src/PlayerStanding/player_standings.xlsx
+++ b/src/PlayerStanding/player_standings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IIT\1st Year\2nd Trimester\CM1601 [PRO] Programming Fundamentals\CW\fx\src\PlayerStanding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{6F798DC0-848A-4B17-8210-BB5677C029CB}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{6EE27711-BCEC-405B-8854-883EA735EE95}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView windowHeight="12855" windowWidth="21600" xWindow="7620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="2280"/>
+    <workbookView windowHeight="12855" windowWidth="21600" xWindow="3375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="1065"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
   <si>
     <t>PLAYER NAME</t>
   </si>
@@ -160,9 +160,6 @@
     <t>Jasprit Bumrah</t>
   </si>
   <si>
-    <t>Kuldeep</t>
-  </si>
-  <si>
     <t>Mohammad Rizwan</t>
   </si>
   <si>
@@ -293,6 +290,12 @@
   </si>
   <si>
     <t>Nuwan Pradeep</t>
+  </si>
+  <si>
+    <t>Kuldeep Yadav</t>
+  </si>
+  <si>
+    <t>GOTA</t>
   </si>
 </sst>
 </file>
@@ -697,11 +700,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="E87" sqref="E87"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -718,8 +724,8 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="n">
-        <v>41.0</v>
+      <c r="B2">
+        <v>101</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -729,8 +735,8 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="n">
-        <v>99.0</v>
+      <c r="B3">
+        <v>212</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -740,8 +746,8 @@
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="n">
-        <v>42.0</v>
+      <c r="B4">
+        <v>250</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -751,8 +757,8 @@
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="n">
-        <v>65.0</v>
+      <c r="B5">
+        <v>150</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -762,8 +768,8 @@
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="n">
-        <v>31.0</v>
+      <c r="B6">
+        <v>157</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -773,8 +779,8 @@
       <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" t="n">
-        <v>55.0</v>
+      <c r="B7">
+        <v>233</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -784,55 +790,55 @@
       <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" t="n">
-        <v>22.0</v>
-      </c>
-      <c r="C8" t="n">
-        <v>4.0</v>
+      <c r="B8">
+        <v>60</v>
+      </c>
+      <c r="C8">
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B9" t="n">
-        <v>48.0</v>
-      </c>
-      <c r="C9" t="n">
-        <v>5.0</v>
+      <c r="B9">
+        <v>155</v>
+      </c>
+      <c r="C9">
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="B10" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="C10" t="n">
-        <v>2.0</v>
+      <c r="B10">
+        <v>138</v>
+      </c>
+      <c r="C10">
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B11" t="n">
-        <v>13.0</v>
-      </c>
-      <c r="C11" t="n">
-        <v>3.0</v>
+      <c r="B11">
+        <v>71</v>
+      </c>
+      <c r="C11">
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B12" t="n">
-        <v>11.0</v>
-      </c>
-      <c r="C12" t="n">
-        <v>6.0</v>
+      <c r="B12">
+        <v>94</v>
+      </c>
+      <c r="C12">
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -840,7 +846,7 @@
         <v>14</v>
       </c>
       <c r="B13" t="n">
-        <v>51.0</v>
+        <v>205.0</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -851,7 +857,7 @@
         <v>15</v>
       </c>
       <c r="B14" t="n">
-        <v>59.0</v>
+        <v>152.0</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -862,7 +868,7 @@
         <v>16</v>
       </c>
       <c r="B15" t="n">
-        <v>90.0</v>
+        <v>185.0</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -873,7 +879,7 @@
         <v>17</v>
       </c>
       <c r="B16" t="n">
-        <v>38.0</v>
+        <v>199.0</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -884,7 +890,7 @@
         <v>18</v>
       </c>
       <c r="B17" t="n">
-        <v>11.0</v>
+        <v>55.0</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -895,7 +901,7 @@
         <v>19</v>
       </c>
       <c r="B18" t="n">
-        <v>25.0</v>
+        <v>148.0</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -906,10 +912,10 @@
         <v>20</v>
       </c>
       <c r="B19" t="n">
-        <v>97.0</v>
+        <v>208.0</v>
       </c>
       <c r="C19" t="n">
-        <v>5.0</v>
+        <v>22.0</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -917,10 +923,10 @@
         <v>21</v>
       </c>
       <c r="B20" t="n">
-        <v>22.0</v>
+        <v>136.0</v>
       </c>
       <c r="C20" t="n">
-        <v>4.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -928,10 +934,10 @@
         <v>22</v>
       </c>
       <c r="B21" t="n">
-        <v>49.0</v>
+        <v>100.0</v>
       </c>
       <c r="C21" t="n">
-        <v>7.0</v>
+        <v>20.0</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -939,10 +945,10 @@
         <v>23</v>
       </c>
       <c r="B22" t="n">
-        <v>9.0</v>
+        <v>59.0</v>
       </c>
       <c r="C22" t="n">
-        <v>5.0</v>
+        <v>19.0</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -950,18 +956,18 @@
         <v>24</v>
       </c>
       <c r="B23" t="n">
-        <v>22.0</v>
+        <v>60.0</v>
       </c>
       <c r="C23" t="n">
-        <v>9.0</v>
+        <v>24.0</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>25</v>
       </c>
-      <c r="B24" t="n">
-        <v>118.0</v>
+      <c r="B24">
+        <v>127</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -971,8 +977,8 @@
       <c r="A25" t="s">
         <v>26</v>
       </c>
-      <c r="B25" t="n">
-        <v>67.0</v>
+      <c r="B25">
+        <v>83</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -982,8 +988,8 @@
       <c r="A26" t="s">
         <v>27</v>
       </c>
-      <c r="B26" t="n">
-        <v>120.0</v>
+      <c r="B26">
+        <v>158</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -993,8 +999,8 @@
       <c r="A27" t="s">
         <v>28</v>
       </c>
-      <c r="B27" t="n">
-        <v>54.0</v>
+      <c r="B27">
+        <v>56</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -1004,8 +1010,8 @@
       <c r="A28" t="s">
         <v>29</v>
       </c>
-      <c r="B28" t="n">
-        <v>42.0</v>
+      <c r="B28">
+        <v>50</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -1015,8 +1021,8 @@
       <c r="A29" t="s">
         <v>30</v>
       </c>
-      <c r="B29" t="n">
-        <v>81.0</v>
+      <c r="B29">
+        <v>104</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -1026,55 +1032,55 @@
       <c r="A30" t="s">
         <v>31</v>
       </c>
-      <c r="B30" t="n">
-        <v>47.0</v>
-      </c>
-      <c r="C30" t="n">
-        <v>11.0</v>
+      <c r="B30">
+        <v>115</v>
+      </c>
+      <c r="C30">
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>32</v>
       </c>
-      <c r="B31" t="n">
-        <v>78.0</v>
-      </c>
-      <c r="C31" t="n">
-        <v>3.0</v>
+      <c r="B31">
+        <v>90</v>
+      </c>
+      <c r="C31">
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>33</v>
       </c>
-      <c r="B32" t="n">
-        <v>36.0</v>
-      </c>
-      <c r="C32" t="n">
-        <v>3.0</v>
+      <c r="B32">
+        <v>62</v>
+      </c>
+      <c r="C32">
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>34</v>
       </c>
-      <c r="B33" t="n">
-        <v>25.0</v>
-      </c>
-      <c r="C33" t="n">
-        <v>9.0</v>
+      <c r="B33">
+        <v>89</v>
+      </c>
+      <c r="C33">
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>35</v>
       </c>
-      <c r="B34" t="n">
-        <v>17.0</v>
-      </c>
-      <c r="C34" t="n">
-        <v>4.0</v>
+      <c r="B34">
+        <v>19</v>
+      </c>
+      <c r="C34">
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1082,7 +1088,7 @@
         <v>36</v>
       </c>
       <c r="B35" t="n">
-        <v>47.0</v>
+        <v>137.0</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -1093,7 +1099,7 @@
         <v>37</v>
       </c>
       <c r="B36" t="n">
-        <v>2.0</v>
+        <v>86.0</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -1104,7 +1110,7 @@
         <v>38</v>
       </c>
       <c r="B37" t="n">
-        <v>35.0</v>
+        <v>107.0</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -1115,7 +1121,7 @@
         <v>39</v>
       </c>
       <c r="B38" t="n">
-        <v>71.0</v>
+        <v>166.0</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -1126,7 +1132,7 @@
         <v>40</v>
       </c>
       <c r="B39" t="n">
-        <v>65.0</v>
+        <v>166.0</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -1137,7 +1143,7 @@
         <v>41</v>
       </c>
       <c r="B40" t="n">
-        <v>31.0</v>
+        <v>69.0</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -1148,10 +1154,10 @@
         <v>42</v>
       </c>
       <c r="B41" t="n">
-        <v>15.0</v>
+        <v>111.0</v>
       </c>
       <c r="C41" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1159,10 +1165,10 @@
         <v>43</v>
       </c>
       <c r="B42" t="n">
-        <v>24.0</v>
+        <v>50.0</v>
       </c>
       <c r="C42" t="n">
-        <v>3.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1170,10 +1176,10 @@
         <v>44</v>
       </c>
       <c r="B43" t="n">
-        <v>22.0</v>
+        <v>66.0</v>
       </c>
       <c r="C43" t="n">
-        <v>3.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1181,29 +1187,29 @@
         <v>45</v>
       </c>
       <c r="B44" t="n">
-        <v>20.0</v>
+        <v>72.0</v>
       </c>
       <c r="C44" t="n">
-        <v>7.0</v>
+        <v>14.0</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>46</v>
+        <v>91</v>
       </c>
       <c r="B45" t="n">
-        <v>32.0</v>
+        <v>46.0</v>
       </c>
       <c r="C45" t="n">
-        <v>7.0</v>
+        <v>19.0</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>47</v>
-      </c>
-      <c r="B46" t="n">
-        <v>183.0</v>
+        <v>46</v>
+      </c>
+      <c r="B46">
+        <v>299</v>
       </c>
       <c r="C46">
         <v>0</v>
@@ -1211,10 +1217,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>48</v>
-      </c>
-      <c r="B47" t="n">
-        <v>147.0</v>
+        <v>47</v>
+      </c>
+      <c r="B47">
+        <v>210</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -1222,10 +1228,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>49</v>
-      </c>
-      <c r="B48" t="n">
-        <v>86.0</v>
+        <v>48</v>
+      </c>
+      <c r="B48">
+        <v>109</v>
       </c>
       <c r="C48">
         <v>0</v>
@@ -1233,10 +1239,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>50</v>
-      </c>
-      <c r="B49" t="n">
-        <v>87.0</v>
+        <v>49</v>
+      </c>
+      <c r="B49">
+        <v>129</v>
       </c>
       <c r="C49">
         <v>0</v>
@@ -1244,10 +1250,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>51</v>
-      </c>
-      <c r="B50" t="n">
-        <v>142.0</v>
+        <v>50</v>
+      </c>
+      <c r="B50">
+        <v>205</v>
       </c>
       <c r="C50">
         <v>0</v>
@@ -1255,10 +1261,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>52</v>
-      </c>
-      <c r="B51" t="n">
-        <v>113.0</v>
+        <v>51</v>
+      </c>
+      <c r="B51">
+        <v>138</v>
       </c>
       <c r="C51">
         <v>0</v>
@@ -1266,65 +1272,65 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>53</v>
-      </c>
-      <c r="B52" t="n">
-        <v>141.0</v>
-      </c>
-      <c r="C52" t="n">
-        <v>14.0</v>
+        <v>52</v>
+      </c>
+      <c r="B52">
+        <v>188</v>
+      </c>
+      <c r="C52">
+        <v>17</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>54</v>
-      </c>
-      <c r="B53" t="n">
-        <v>82.0</v>
-      </c>
-      <c r="C53" t="n">
-        <v>13.0</v>
+        <v>53</v>
+      </c>
+      <c r="B53">
+        <v>91</v>
+      </c>
+      <c r="C53">
+        <v>14</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>55</v>
-      </c>
-      <c r="B54" t="n">
-        <v>26.0</v>
-      </c>
-      <c r="C54" t="n">
-        <v>12.0</v>
+        <v>54</v>
+      </c>
+      <c r="B54">
+        <v>80</v>
+      </c>
+      <c r="C54">
+        <v>17</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>56</v>
-      </c>
-      <c r="B55" t="n">
-        <v>104.0</v>
-      </c>
-      <c r="C55" t="n">
-        <v>20.0</v>
+        <v>55</v>
+      </c>
+      <c r="B55">
+        <v>122</v>
+      </c>
+      <c r="C55">
+        <v>28</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>57</v>
-      </c>
-      <c r="B56" t="n">
-        <v>89.0</v>
-      </c>
-      <c r="C56" t="n">
-        <v>22.0</v>
+        <v>56</v>
+      </c>
+      <c r="B56">
+        <v>104</v>
+      </c>
+      <c r="C56">
+        <v>27</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>58</v>
-      </c>
-      <c r="B57" t="n">
-        <v>134.0</v>
+        <v>57</v>
+      </c>
+      <c r="B57">
+        <v>134</v>
       </c>
       <c r="C57">
         <v>0</v>
@@ -1332,10 +1338,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>59</v>
-      </c>
-      <c r="B58" t="n">
-        <v>78.0</v>
+        <v>58</v>
+      </c>
+      <c r="B58">
+        <v>78</v>
       </c>
       <c r="C58">
         <v>0</v>
@@ -1343,10 +1349,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>60</v>
-      </c>
-      <c r="B59" t="n">
-        <v>81.0</v>
+        <v>59</v>
+      </c>
+      <c r="B59">
+        <v>81</v>
       </c>
       <c r="C59">
         <v>0</v>
@@ -1354,10 +1360,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>61</v>
-      </c>
-      <c r="B60" t="n">
-        <v>40.0</v>
+        <v>60</v>
+      </c>
+      <c r="B60">
+        <v>40</v>
       </c>
       <c r="C60">
         <v>0</v>
@@ -1365,10 +1371,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>62</v>
-      </c>
-      <c r="B61" t="n">
-        <v>101.0</v>
+        <v>61</v>
+      </c>
+      <c r="B61">
+        <v>101</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -1376,10 +1382,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>63</v>
-      </c>
-      <c r="B62" t="n">
-        <v>90.0</v>
+        <v>62</v>
+      </c>
+      <c r="B62">
+        <v>90</v>
       </c>
       <c r="C62">
         <v>0</v>
@@ -1387,65 +1393,65 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>64</v>
-      </c>
-      <c r="B63" t="n">
-        <v>58.0</v>
-      </c>
-      <c r="C63" t="n">
-        <v>8.0</v>
+        <v>63</v>
+      </c>
+      <c r="B63">
+        <v>58</v>
+      </c>
+      <c r="C63">
+        <v>8</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>65</v>
-      </c>
-      <c r="B64" t="n">
-        <v>36.0</v>
-      </c>
-      <c r="C64" t="n">
-        <v>7.0</v>
+        <v>64</v>
+      </c>
+      <c r="B64">
+        <v>36</v>
+      </c>
+      <c r="C64">
+        <v>7</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>66</v>
-      </c>
-      <c r="B65" t="n">
-        <v>25.0</v>
-      </c>
-      <c r="C65" t="n">
-        <v>7.0</v>
+        <v>65</v>
+      </c>
+      <c r="B65">
+        <v>25</v>
+      </c>
+      <c r="C65">
+        <v>7</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>67</v>
-      </c>
-      <c r="B66" t="n">
-        <v>33.0</v>
-      </c>
-      <c r="C66" t="n">
-        <v>13.0</v>
+        <v>66</v>
+      </c>
+      <c r="B66">
+        <v>33</v>
+      </c>
+      <c r="C66">
+        <v>13</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>68</v>
-      </c>
-      <c r="B67" t="n">
-        <v>14.0</v>
-      </c>
-      <c r="C67" t="n">
-        <v>15.0</v>
+        <v>67</v>
+      </c>
+      <c r="B67">
+        <v>14</v>
+      </c>
+      <c r="C67">
+        <v>15</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>69</v>
-      </c>
-      <c r="B68" t="n">
-        <v>26.0</v>
+        <v>68</v>
+      </c>
+      <c r="B68">
+        <v>35</v>
       </c>
       <c r="C68">
         <v>0</v>
@@ -1453,10 +1459,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>70</v>
-      </c>
-      <c r="B69" t="n">
-        <v>42.0</v>
+        <v>69</v>
+      </c>
+      <c r="B69">
+        <v>73</v>
       </c>
       <c r="C69">
         <v>0</v>
@@ -1464,10 +1470,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>71</v>
-      </c>
-      <c r="B70" t="n">
-        <v>88.0</v>
+        <v>70</v>
+      </c>
+      <c r="B70">
+        <v>144</v>
       </c>
       <c r="C70">
         <v>0</v>
@@ -1475,10 +1481,10 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>72</v>
-      </c>
-      <c r="B71" t="n">
-        <v>16.0</v>
+        <v>71</v>
+      </c>
+      <c r="B71">
+        <v>134</v>
       </c>
       <c r="C71">
         <v>0</v>
@@ -1486,10 +1492,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>73</v>
-      </c>
-      <c r="B72" t="n">
-        <v>15.0</v>
+        <v>72</v>
+      </c>
+      <c r="B72">
+        <v>63</v>
       </c>
       <c r="C72">
         <v>0</v>
@@ -1497,10 +1503,10 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>74</v>
-      </c>
-      <c r="B73" t="n">
-        <v>45.0</v>
+        <v>73</v>
+      </c>
+      <c r="B73">
+        <v>150</v>
       </c>
       <c r="C73">
         <v>0</v>
@@ -1508,65 +1514,65 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>75</v>
-      </c>
-      <c r="B74" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="C74" t="n">
-        <v>3.0</v>
+        <v>74</v>
+      </c>
+      <c r="B74">
+        <v>97</v>
+      </c>
+      <c r="C74">
+        <v>9</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>76</v>
-      </c>
-      <c r="B75" t="n">
-        <v>30.0</v>
-      </c>
-      <c r="C75" t="n">
-        <v>4.0</v>
+        <v>75</v>
+      </c>
+      <c r="B75">
+        <v>90</v>
+      </c>
+      <c r="C75">
+        <v>11</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>77</v>
-      </c>
-      <c r="B76" t="n">
-        <v>33.0</v>
-      </c>
-      <c r="C76" t="n">
-        <v>4.0</v>
+        <v>76</v>
+      </c>
+      <c r="B76">
+        <v>63</v>
+      </c>
+      <c r="C76">
+        <v>9</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>78</v>
-      </c>
-      <c r="B77" t="n">
-        <v>18.0</v>
-      </c>
-      <c r="C77" t="n">
-        <v>4.0</v>
+        <v>77</v>
+      </c>
+      <c r="B77">
+        <v>33</v>
+      </c>
+      <c r="C77">
+        <v>14</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>79</v>
-      </c>
-      <c r="B78" t="n">
-        <v>16.0</v>
-      </c>
-      <c r="C78" t="n">
-        <v>5.0</v>
+        <v>78</v>
+      </c>
+      <c r="B78">
+        <v>20</v>
+      </c>
+      <c r="C78">
+        <v>12</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>80</v>
-      </c>
-      <c r="B79" t="n">
-        <v>32.0</v>
+        <v>79</v>
+      </c>
+      <c r="B79">
+        <v>102</v>
       </c>
       <c r="C79">
         <v>0</v>
@@ -1574,10 +1580,10 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>81</v>
-      </c>
-      <c r="B80" t="n">
-        <v>89.0</v>
+        <v>80</v>
+      </c>
+      <c r="B80">
+        <v>193</v>
       </c>
       <c r="C80">
         <v>0</v>
@@ -1585,21 +1591,21 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>82</v>
-      </c>
-      <c r="B81" t="n">
-        <v>93.0</v>
+        <v>81</v>
+      </c>
+      <c r="B81">
+        <v>189</v>
       </c>
       <c r="C81">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>83</v>
-      </c>
-      <c r="B82" t="n">
-        <v>126.0</v>
+        <v>82</v>
+      </c>
+      <c r="B82">
+        <v>157</v>
       </c>
       <c r="C82">
         <v>0</v>
@@ -1607,10 +1613,10 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>84</v>
-      </c>
-      <c r="B83" t="n">
-        <v>69.0</v>
+        <v>83</v>
+      </c>
+      <c r="B83">
+        <v>69</v>
       </c>
       <c r="C83">
         <v>0</v>
@@ -1618,10 +1624,10 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>85</v>
-      </c>
-      <c r="B84" t="n">
-        <v>54.0</v>
+        <v>84</v>
+      </c>
+      <c r="B84">
+        <v>67</v>
       </c>
       <c r="C84">
         <v>0</v>
@@ -1629,57 +1635,57 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>86</v>
-      </c>
-      <c r="B85" t="n">
-        <v>94.0</v>
-      </c>
-      <c r="C85" t="n">
-        <v>5.0</v>
+        <v>85</v>
+      </c>
+      <c r="B85">
+        <v>102</v>
+      </c>
+      <c r="C85">
+        <v>9</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>87</v>
-      </c>
-      <c r="B86" t="n">
-        <v>13.0</v>
-      </c>
-      <c r="C86" t="n">
-        <v>3.0</v>
+        <v>86</v>
+      </c>
+      <c r="B86">
+        <v>36</v>
+      </c>
+      <c r="C86">
+        <v>10</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>88</v>
-      </c>
-      <c r="B87" t="n">
-        <v>72.0</v>
-      </c>
-      <c r="C87" t="n">
-        <v>7.0</v>
+        <v>87</v>
+      </c>
+      <c r="B87">
+        <v>122</v>
+      </c>
+      <c r="C87">
+        <v>14</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>89</v>
-      </c>
-      <c r="B88" t="n">
-        <v>53.0</v>
-      </c>
-      <c r="C88" t="n">
-        <v>6.0</v>
+        <v>88</v>
+      </c>
+      <c r="B88">
+        <v>70</v>
+      </c>
+      <c r="C88">
+        <v>14</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>90</v>
-      </c>
-      <c r="B89" t="n">
-        <v>74.0</v>
-      </c>
-      <c r="C89" t="n">
-        <v>9.0</v>
+        <v>89</v>
+      </c>
+      <c r="B89">
+        <v>87</v>
+      </c>
+      <c r="C89">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
team profile edit done
</commit_message>
<xml_diff>
--- a/src/PlayerStanding/player_standings.xlsx
+++ b/src/PlayerStanding/player_standings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IIT\1st Year\2nd Trimester\CM1601 [PRO] Programming Fundamentals\CW\fx\src\PlayerStanding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{6EE27711-BCEC-405B-8854-883EA735EE95}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{786920F9-90F1-4134-A616-F71322D626E7}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView windowHeight="12855" windowWidth="21600" xWindow="3375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="1065"/>
+    <workbookView windowHeight="7995" windowWidth="15375" xWindow="1170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="1620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
   <si>
     <t>PLAYER NAME</t>
   </si>
@@ -290,9 +290,6 @@
   </si>
   <si>
     <t>Nuwan Pradeep</t>
-  </si>
-  <si>
-    <t>Kuldeep Yadav</t>
   </si>
   <si>
     <t>GOTA</t>
@@ -700,8 +697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -724,8 +721,8 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
-        <v>101</v>
+      <c r="B2" t="n">
+        <v>7.0</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -735,8 +732,8 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
-        <v>212</v>
+      <c r="B3" t="n">
+        <v>34.0</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -746,8 +743,8 @@
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
-        <v>250</v>
+      <c r="B4" t="n">
+        <v>52.0</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -757,8 +754,8 @@
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5">
-        <v>150</v>
+      <c r="B5" t="n">
+        <v>39.0</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -768,8 +765,8 @@
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6">
-        <v>157</v>
+      <c r="B6" t="n">
+        <v>17.0</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -779,8 +776,8 @@
       <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B7">
-        <v>233</v>
+      <c r="B7" t="n">
+        <v>15.0</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -790,55 +787,55 @@
       <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B8">
-        <v>60</v>
-      </c>
-      <c r="C8">
-        <v>12</v>
+      <c r="B8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>2.0</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B9">
-        <v>155</v>
-      </c>
-      <c r="C9">
-        <v>12</v>
+      <c r="B9" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1.0</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="B10">
-        <v>138</v>
-      </c>
-      <c r="C10">
-        <v>13</v>
+      <c r="B10" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>2.0</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B11">
-        <v>71</v>
-      </c>
-      <c r="C11">
-        <v>13</v>
+      <c r="B11" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>2.0</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B12">
-        <v>94</v>
-      </c>
-      <c r="C12">
-        <v>17</v>
+      <c r="B12" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>3.0</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -846,7 +843,7 @@
         <v>14</v>
       </c>
       <c r="B13" t="n">
-        <v>205.0</v>
+        <v>36.0</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -857,7 +854,7 @@
         <v>15</v>
       </c>
       <c r="B14" t="n">
-        <v>152.0</v>
+        <v>2.0</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -868,7 +865,7 @@
         <v>16</v>
       </c>
       <c r="B15" t="n">
-        <v>185.0</v>
+        <v>0.0</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -879,7 +876,7 @@
         <v>17</v>
       </c>
       <c r="B16" t="n">
-        <v>199.0</v>
+        <v>64.0</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -890,7 +887,7 @@
         <v>18</v>
       </c>
       <c r="B17" t="n">
-        <v>55.0</v>
+        <v>26.0</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -901,7 +898,7 @@
         <v>19</v>
       </c>
       <c r="B18" t="n">
-        <v>148.0</v>
+        <v>2.0</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -912,10 +909,10 @@
         <v>20</v>
       </c>
       <c r="B19" t="n">
-        <v>208.0</v>
+        <v>17.0</v>
       </c>
       <c r="C19" t="n">
-        <v>22.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -923,10 +920,10 @@
         <v>21</v>
       </c>
       <c r="B20" t="n">
-        <v>136.0</v>
+        <v>25.0</v>
       </c>
       <c r="C20" t="n">
-        <v>12.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -934,10 +931,10 @@
         <v>22</v>
       </c>
       <c r="B21" t="n">
-        <v>100.0</v>
+        <v>37.0</v>
       </c>
       <c r="C21" t="n">
-        <v>20.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -945,10 +942,10 @@
         <v>23</v>
       </c>
       <c r="B22" t="n">
-        <v>59.0</v>
+        <v>0.0</v>
       </c>
       <c r="C22" t="n">
-        <v>19.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -956,10 +953,10 @@
         <v>24</v>
       </c>
       <c r="B23" t="n">
-        <v>60.0</v>
+        <v>3.0</v>
       </c>
       <c r="C23" t="n">
-        <v>24.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -967,7 +964,7 @@
         <v>25</v>
       </c>
       <c r="B24">
-        <v>127</v>
+        <v>0</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -978,7 +975,7 @@
         <v>26</v>
       </c>
       <c r="B25">
-        <v>83</v>
+        <v>0</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -989,7 +986,7 @@
         <v>27</v>
       </c>
       <c r="B26">
-        <v>158</v>
+        <v>0</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -1000,7 +997,7 @@
         <v>28</v>
       </c>
       <c r="B27">
-        <v>56</v>
+        <v>0</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -1011,7 +1008,7 @@
         <v>29</v>
       </c>
       <c r="B28">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -1022,7 +1019,7 @@
         <v>30</v>
       </c>
       <c r="B29">
-        <v>104</v>
+        <v>0</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -1033,10 +1030,10 @@
         <v>31</v>
       </c>
       <c r="B30">
-        <v>115</v>
+        <v>0</v>
       </c>
       <c r="C30">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -1044,10 +1041,10 @@
         <v>32</v>
       </c>
       <c r="B31">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="C31">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1055,10 +1052,10 @@
         <v>33</v>
       </c>
       <c r="B32">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="C32">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1066,10 +1063,10 @@
         <v>34</v>
       </c>
       <c r="B33">
-        <v>89</v>
+        <v>0</v>
       </c>
       <c r="C33">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -1077,18 +1074,18 @@
         <v>35</v>
       </c>
       <c r="B34">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="C34">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>36</v>
       </c>
-      <c r="B35" t="n">
-        <v>137.0</v>
+      <c r="B35">
+        <v>0</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -1098,8 +1095,8 @@
       <c r="A36" t="s">
         <v>37</v>
       </c>
-      <c r="B36" t="n">
-        <v>86.0</v>
+      <c r="B36">
+        <v>0</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -1109,8 +1106,8 @@
       <c r="A37" t="s">
         <v>38</v>
       </c>
-      <c r="B37" t="n">
-        <v>107.0</v>
+      <c r="B37">
+        <v>0</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -1120,8 +1117,8 @@
       <c r="A38" t="s">
         <v>39</v>
       </c>
-      <c r="B38" t="n">
-        <v>166.0</v>
+      <c r="B38">
+        <v>0</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -1131,8 +1128,8 @@
       <c r="A39" t="s">
         <v>40</v>
       </c>
-      <c r="B39" t="n">
-        <v>166.0</v>
+      <c r="B39">
+        <v>0</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -1142,8 +1139,8 @@
       <c r="A40" t="s">
         <v>41</v>
       </c>
-      <c r="B40" t="n">
-        <v>69.0</v>
+      <c r="B40">
+        <v>0</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -1153,55 +1150,55 @@
       <c r="A41" t="s">
         <v>42</v>
       </c>
-      <c r="B41" t="n">
-        <v>111.0</v>
-      </c>
-      <c r="C41" t="n">
-        <v>5.0</v>
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>43</v>
       </c>
-      <c r="B42" t="n">
-        <v>50.0</v>
-      </c>
-      <c r="C42" t="n">
-        <v>13.0</v>
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>44</v>
       </c>
-      <c r="B43" t="n">
-        <v>66.0</v>
-      </c>
-      <c r="C43" t="n">
-        <v>7.0</v>
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>45</v>
       </c>
-      <c r="B44" t="n">
-        <v>72.0</v>
-      </c>
-      <c r="C44" t="n">
-        <v>14.0</v>
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>91</v>
-      </c>
-      <c r="B45" t="n">
-        <v>46.0</v>
-      </c>
-      <c r="C45" t="n">
-        <v>19.0</v>
+        <v>90</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1209,7 +1206,7 @@
         <v>46</v>
       </c>
       <c r="B46">
-        <v>299</v>
+        <v>0</v>
       </c>
       <c r="C46">
         <v>0</v>
@@ -1220,7 +1217,7 @@
         <v>47</v>
       </c>
       <c r="B47">
-        <v>210</v>
+        <v>0</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -1231,7 +1228,7 @@
         <v>48</v>
       </c>
       <c r="B48">
-        <v>109</v>
+        <v>0</v>
       </c>
       <c r="C48">
         <v>0</v>
@@ -1242,7 +1239,7 @@
         <v>49</v>
       </c>
       <c r="B49">
-        <v>129</v>
+        <v>0</v>
       </c>
       <c r="C49">
         <v>0</v>
@@ -1253,7 +1250,7 @@
         <v>50</v>
       </c>
       <c r="B50">
-        <v>205</v>
+        <v>0</v>
       </c>
       <c r="C50">
         <v>0</v>
@@ -1264,7 +1261,7 @@
         <v>51</v>
       </c>
       <c r="B51">
-        <v>138</v>
+        <v>0</v>
       </c>
       <c r="C51">
         <v>0</v>
@@ -1275,10 +1272,10 @@
         <v>52</v>
       </c>
       <c r="B52">
-        <v>188</v>
+        <v>0</v>
       </c>
       <c r="C52">
-        <v>17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1286,10 +1283,10 @@
         <v>53</v>
       </c>
       <c r="B53">
-        <v>91</v>
+        <v>0</v>
       </c>
       <c r="C53">
-        <v>14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -1297,10 +1294,10 @@
         <v>54</v>
       </c>
       <c r="B54">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="C54">
-        <v>17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -1308,10 +1305,10 @@
         <v>55</v>
       </c>
       <c r="B55">
-        <v>122</v>
+        <v>0</v>
       </c>
       <c r="C55">
-        <v>28</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -1319,10 +1316,10 @@
         <v>56</v>
       </c>
       <c r="B56">
-        <v>104</v>
+        <v>0</v>
       </c>
       <c r="C56">
-        <v>27</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -1330,7 +1327,7 @@
         <v>57</v>
       </c>
       <c r="B57">
-        <v>134</v>
+        <v>0</v>
       </c>
       <c r="C57">
         <v>0</v>
@@ -1341,7 +1338,7 @@
         <v>58</v>
       </c>
       <c r="B58">
-        <v>78</v>
+        <v>0</v>
       </c>
       <c r="C58">
         <v>0</v>
@@ -1352,7 +1349,7 @@
         <v>59</v>
       </c>
       <c r="B59">
-        <v>81</v>
+        <v>0</v>
       </c>
       <c r="C59">
         <v>0</v>
@@ -1363,7 +1360,7 @@
         <v>60</v>
       </c>
       <c r="B60">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="C60">
         <v>0</v>
@@ -1374,7 +1371,7 @@
         <v>61</v>
       </c>
       <c r="B61">
-        <v>101</v>
+        <v>0</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -1385,7 +1382,7 @@
         <v>62</v>
       </c>
       <c r="B62">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="C62">
         <v>0</v>
@@ -1396,10 +1393,10 @@
         <v>63</v>
       </c>
       <c r="B63">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="C63">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -1407,10 +1404,10 @@
         <v>64</v>
       </c>
       <c r="B64">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="C64">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -1418,10 +1415,10 @@
         <v>65</v>
       </c>
       <c r="B65">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="C65">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -1429,10 +1426,10 @@
         <v>66</v>
       </c>
       <c r="B66">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="C66">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -1440,10 +1437,10 @@
         <v>67</v>
       </c>
       <c r="B67">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C67">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -1451,7 +1448,7 @@
         <v>68</v>
       </c>
       <c r="B68">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="C68">
         <v>0</v>
@@ -1462,7 +1459,7 @@
         <v>69</v>
       </c>
       <c r="B69">
-        <v>73</v>
+        <v>0</v>
       </c>
       <c r="C69">
         <v>0</v>
@@ -1473,7 +1470,7 @@
         <v>70</v>
       </c>
       <c r="B70">
-        <v>144</v>
+        <v>0</v>
       </c>
       <c r="C70">
         <v>0</v>
@@ -1484,7 +1481,7 @@
         <v>71</v>
       </c>
       <c r="B71">
-        <v>134</v>
+        <v>0</v>
       </c>
       <c r="C71">
         <v>0</v>
@@ -1495,7 +1492,7 @@
         <v>72</v>
       </c>
       <c r="B72">
-        <v>63</v>
+        <v>0</v>
       </c>
       <c r="C72">
         <v>0</v>
@@ -1506,7 +1503,7 @@
         <v>73</v>
       </c>
       <c r="B73">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="C73">
         <v>0</v>
@@ -1517,10 +1514,10 @@
         <v>74</v>
       </c>
       <c r="B74">
-        <v>97</v>
+        <v>0</v>
       </c>
       <c r="C74">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -1528,10 +1525,10 @@
         <v>75</v>
       </c>
       <c r="B75">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="C75">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -1539,10 +1536,10 @@
         <v>76</v>
       </c>
       <c r="B76">
-        <v>63</v>
+        <v>0</v>
       </c>
       <c r="C76">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -1550,10 +1547,10 @@
         <v>77</v>
       </c>
       <c r="B77">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="C77">
-        <v>14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -1561,10 +1558,10 @@
         <v>78</v>
       </c>
       <c r="B78">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C78">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -1572,7 +1569,7 @@
         <v>79</v>
       </c>
       <c r="B79">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="C79">
         <v>0</v>
@@ -1583,7 +1580,7 @@
         <v>80</v>
       </c>
       <c r="B80">
-        <v>193</v>
+        <v>0</v>
       </c>
       <c r="C80">
         <v>0</v>
@@ -1594,10 +1591,10 @@
         <v>81</v>
       </c>
       <c r="B81">
-        <v>189</v>
+        <v>0</v>
       </c>
       <c r="C81">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -1605,7 +1602,7 @@
         <v>82</v>
       </c>
       <c r="B82">
-        <v>157</v>
+        <v>0</v>
       </c>
       <c r="C82">
         <v>0</v>
@@ -1616,7 +1613,7 @@
         <v>83</v>
       </c>
       <c r="B83">
-        <v>69</v>
+        <v>0</v>
       </c>
       <c r="C83">
         <v>0</v>
@@ -1627,7 +1624,7 @@
         <v>84</v>
       </c>
       <c r="B84">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="C84">
         <v>0</v>
@@ -1638,10 +1635,10 @@
         <v>85</v>
       </c>
       <c r="B85">
-        <v>102</v>
+        <v>0</v>
       </c>
       <c r="C85">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -1649,10 +1646,10 @@
         <v>86</v>
       </c>
       <c r="B86">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="C86">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -1660,10 +1657,10 @@
         <v>87</v>
       </c>
       <c r="B87">
-        <v>122</v>
+        <v>0</v>
       </c>
       <c r="C87">
-        <v>14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -1671,10 +1668,10 @@
         <v>88</v>
       </c>
       <c r="B88">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="C88">
-        <v>14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -1682,10 +1679,10 @@
         <v>89</v>
       </c>
       <c r="B89">
-        <v>87</v>
+        <v>0</v>
       </c>
       <c r="C89">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cw done final commit
</commit_message>
<xml_diff>
--- a/src/PlayerStanding/player_standings.xlsx
+++ b/src/PlayerStanding/player_standings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IIT\1st Year\2nd Trimester\CM1601 [PRO] Programming Fundamentals\CW\fx\src\PlayerStanding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{786920F9-90F1-4134-A616-F71322D626E7}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{2BE690FD-CB94-4302-BE46-312666E0BF33}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView windowHeight="7995" windowWidth="15375" xWindow="1170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="1620"/>
+    <workbookView windowHeight="12855" windowWidth="21600" xWindow="2340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="2790"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
   <si>
     <t>PLAYER NAME</t>
   </si>
@@ -287,12 +287,6 @@
   </si>
   <si>
     <t>Maheesh Theekshana</t>
-  </si>
-  <si>
-    <t>Nuwan Pradeep</t>
-  </si>
-  <si>
-    <t>GOTA</t>
   </si>
   <si>
     <t>Kuldeep Yadav</t>
@@ -704,7 +698,7 @@
   <dimension ref="A1:D89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B2" sqref="B2:C89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,8 +721,8 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="n">
-        <v>687.0</v>
+      <c r="B2">
+        <v>0</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -738,8 +732,8 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="n">
-        <v>747.0</v>
+      <c r="B3">
+        <v>0</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -749,8 +743,8 @@
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="n">
-        <v>725.0</v>
+      <c r="B4">
+        <v>0</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -760,8 +754,8 @@
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="n">
-        <v>639.0</v>
+      <c r="B5">
+        <v>0</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -771,8 +765,8 @@
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="n">
-        <v>650.0</v>
+      <c r="B6">
+        <v>0</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -782,8 +776,8 @@
       <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" t="n">
-        <v>509.0</v>
+      <c r="B7">
+        <v>0</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -793,63 +787,63 @@
       <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" t="n">
-        <v>534.0</v>
-      </c>
-      <c r="C8" t="n">
-        <v>66.0</v>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B9" t="n">
-        <v>379.0</v>
-      </c>
-      <c r="C9" t="n">
-        <v>50.0</v>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="B10" t="n">
-        <v>687.0</v>
-      </c>
-      <c r="C10" t="n">
-        <v>80.0</v>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B11" t="n">
-        <v>328.0</v>
-      </c>
-      <c r="C11" t="n">
-        <v>84.0</v>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B12" t="n">
-        <v>222.0</v>
-      </c>
-      <c r="C12" t="n">
-        <v>88.0</v>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
-      <c r="B13" t="n">
-        <v>845.0</v>
+      <c r="B13">
+        <v>0</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -859,8 +853,8 @@
       <c r="A14" t="s">
         <v>15</v>
       </c>
-      <c r="B14" t="n">
-        <v>774.0</v>
+      <c r="B14">
+        <v>0</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -870,8 +864,8 @@
       <c r="A15" t="s">
         <v>16</v>
       </c>
-      <c r="B15" t="n">
-        <v>608.0</v>
+      <c r="B15">
+        <v>0</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -881,8 +875,8 @@
       <c r="A16" t="s">
         <v>17</v>
       </c>
-      <c r="B16" t="n">
-        <v>686.0</v>
+      <c r="B16">
+        <v>0</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -892,8 +886,8 @@
       <c r="A17" t="s">
         <v>18</v>
       </c>
-      <c r="B17" t="n">
-        <v>532.0</v>
+      <c r="B17">
+        <v>0</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -903,8 +897,8 @@
       <c r="A18" t="s">
         <v>19</v>
       </c>
-      <c r="B18" t="n">
-        <v>603.0</v>
+      <c r="B18">
+        <v>0</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -914,63 +908,63 @@
       <c r="A19" t="s">
         <v>20</v>
       </c>
-      <c r="B19" t="n">
-        <v>734.0</v>
-      </c>
-      <c r="C19" t="n">
-        <v>61.0</v>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>21</v>
       </c>
-      <c r="B20" t="n">
-        <v>619.0</v>
-      </c>
-      <c r="C20" t="n">
-        <v>74.0</v>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
-      <c r="B21" t="n">
-        <v>511.0</v>
-      </c>
-      <c r="C21" t="n">
-        <v>81.0</v>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
-      <c r="B22" t="n">
-        <v>434.0</v>
-      </c>
-      <c r="C22" t="n">
-        <v>82.0</v>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
-      <c r="B23" t="n">
-        <v>366.0</v>
-      </c>
-      <c r="C23" t="n">
-        <v>97.0</v>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>25</v>
       </c>
-      <c r="B24" t="n">
-        <v>811.0</v>
+      <c r="B24">
+        <v>0</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -980,8 +974,8 @@
       <c r="A25" t="s">
         <v>26</v>
       </c>
-      <c r="B25" t="n">
-        <v>756.0</v>
+      <c r="B25">
+        <v>0</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -991,8 +985,8 @@
       <c r="A26" t="s">
         <v>27</v>
       </c>
-      <c r="B26" t="n">
-        <v>708.0</v>
+      <c r="B26">
+        <v>0</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -1002,8 +996,8 @@
       <c r="A27" t="s">
         <v>28</v>
       </c>
-      <c r="B27" t="n">
-        <v>855.0</v>
+      <c r="B27">
+        <v>0</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -1013,8 +1007,8 @@
       <c r="A28" t="s">
         <v>29</v>
       </c>
-      <c r="B28" t="n">
-        <v>771.0</v>
+      <c r="B28">
+        <v>0</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -1024,8 +1018,8 @@
       <c r="A29" t="s">
         <v>30</v>
       </c>
-      <c r="B29" t="n">
-        <v>737.0</v>
+      <c r="B29">
+        <v>0</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -1035,63 +1029,63 @@
       <c r="A30" t="s">
         <v>31</v>
       </c>
-      <c r="B30" t="n">
-        <v>771.0</v>
-      </c>
-      <c r="C30" t="n">
-        <v>52.0</v>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>32</v>
       </c>
-      <c r="B31" t="n">
-        <v>570.0</v>
-      </c>
-      <c r="C31" t="n">
-        <v>70.0</v>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>33</v>
       </c>
-      <c r="B32" t="n">
-        <v>524.0</v>
-      </c>
-      <c r="C32" t="n">
-        <v>92.0</v>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>34</v>
       </c>
-      <c r="B33" t="n">
-        <v>387.0</v>
-      </c>
-      <c r="C33" t="n">
-        <v>90.0</v>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>35</v>
       </c>
-      <c r="B34" t="n">
-        <v>291.0</v>
-      </c>
-      <c r="C34" t="n">
-        <v>99.0</v>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>36</v>
       </c>
-      <c r="B35" t="n">
-        <v>709.0</v>
+      <c r="B35">
+        <v>0</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -1101,8 +1095,8 @@
       <c r="A36" t="s">
         <v>37</v>
       </c>
-      <c r="B36" t="n">
-        <v>393.0</v>
+      <c r="B36">
+        <v>0</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -1112,8 +1106,8 @@
       <c r="A37" t="s">
         <v>38</v>
       </c>
-      <c r="B37" t="n">
-        <v>840.0</v>
+      <c r="B37">
+        <v>0</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -1123,8 +1117,8 @@
       <c r="A38" t="s">
         <v>39</v>
       </c>
-      <c r="B38" t="n">
-        <v>661.0</v>
+      <c r="B38">
+        <v>0</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -1134,8 +1128,8 @@
       <c r="A39" t="s">
         <v>40</v>
       </c>
-      <c r="B39" t="n">
-        <v>625.0</v>
+      <c r="B39">
+        <v>0</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -1145,8 +1139,8 @@
       <c r="A40" t="s">
         <v>41</v>
       </c>
-      <c r="B40" t="n">
-        <v>469.0</v>
+      <c r="B40">
+        <v>0</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -1156,63 +1150,63 @@
       <c r="A41" t="s">
         <v>42</v>
       </c>
-      <c r="B41" t="n">
-        <v>629.0</v>
-      </c>
-      <c r="C41" t="n">
-        <v>46.0</v>
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>43</v>
       </c>
-      <c r="B42" t="n">
-        <v>485.0</v>
-      </c>
-      <c r="C42" t="n">
-        <v>64.0</v>
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>44</v>
       </c>
-      <c r="B43" t="n">
-        <v>510.0</v>
-      </c>
-      <c r="C43" t="n">
-        <v>75.0</v>
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>45</v>
       </c>
-      <c r="B44" t="n">
-        <v>545.0</v>
-      </c>
-      <c r="C44" t="n">
-        <v>81.0</v>
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>91</v>
-      </c>
-      <c r="B45" t="n">
-        <v>346.0</v>
-      </c>
-      <c r="C45" t="n">
-        <v>52.0</v>
+        <v>89</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>46</v>
       </c>
-      <c r="B46" t="n">
-        <v>722.0</v>
+      <c r="B46">
+        <v>0</v>
       </c>
       <c r="C46">
         <v>0</v>
@@ -1222,8 +1216,8 @@
       <c r="A47" t="s">
         <v>47</v>
       </c>
-      <c r="B47" t="n">
-        <v>833.0</v>
+      <c r="B47">
+        <v>0</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -1233,8 +1227,8 @@
       <c r="A48" t="s">
         <v>48</v>
       </c>
-      <c r="B48" t="n">
-        <v>752.0</v>
+      <c r="B48">
+        <v>0</v>
       </c>
       <c r="C48">
         <v>0</v>
@@ -1244,8 +1238,8 @@
       <c r="A49" t="s">
         <v>49</v>
       </c>
-      <c r="B49" t="n">
-        <v>890.0</v>
+      <c r="B49">
+        <v>0</v>
       </c>
       <c r="C49">
         <v>0</v>
@@ -1255,8 +1249,8 @@
       <c r="A50" t="s">
         <v>50</v>
       </c>
-      <c r="B50" t="n">
-        <v>787.0</v>
+      <c r="B50">
+        <v>0</v>
       </c>
       <c r="C50">
         <v>0</v>
@@ -1266,8 +1260,8 @@
       <c r="A51" t="s">
         <v>51</v>
       </c>
-      <c r="B51" t="n">
-        <v>802.0</v>
+      <c r="B51">
+        <v>0</v>
       </c>
       <c r="C51">
         <v>0</v>
@@ -1277,55 +1271,55 @@
       <c r="A52" t="s">
         <v>52</v>
       </c>
-      <c r="B52" t="n">
-        <v>632.0</v>
-      </c>
-      <c r="C52" t="n">
-        <v>76.0</v>
+      <c r="B52">
+        <v>0</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>53</v>
       </c>
-      <c r="B53" t="n">
-        <v>709.0</v>
-      </c>
-      <c r="C53" t="n">
-        <v>58.0</v>
+      <c r="B53">
+        <v>0</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>54</v>
       </c>
-      <c r="B54" t="n">
-        <v>581.0</v>
-      </c>
-      <c r="C54" t="n">
-        <v>81.0</v>
+      <c r="B54">
+        <v>0</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>55</v>
       </c>
-      <c r="B55" t="n">
-        <v>523.0</v>
-      </c>
-      <c r="C55" t="n">
-        <v>90.0</v>
+      <c r="B55">
+        <v>0</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>56</v>
       </c>
-      <c r="B56" t="n">
-        <v>386.0</v>
-      </c>
-      <c r="C56" t="n">
-        <v>92.0</v>
+      <c r="B56">
+        <v>0</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -1333,7 +1327,7 @@
         <v>57</v>
       </c>
       <c r="B57" t="n">
-        <v>801.0</v>
+        <v>55.0</v>
       </c>
       <c r="C57">
         <v>0</v>
@@ -1344,7 +1338,7 @@
         <v>58</v>
       </c>
       <c r="B58" t="n">
-        <v>751.0</v>
+        <v>30.0</v>
       </c>
       <c r="C58">
         <v>0</v>
@@ -1355,7 +1349,7 @@
         <v>59</v>
       </c>
       <c r="B59" t="n">
-        <v>520.0</v>
+        <v>7.0</v>
       </c>
       <c r="C59">
         <v>0</v>
@@ -1366,7 +1360,7 @@
         <v>60</v>
       </c>
       <c r="B60" t="n">
-        <v>542.0</v>
+        <v>18.0</v>
       </c>
       <c r="C60">
         <v>0</v>
@@ -1377,7 +1371,7 @@
         <v>61</v>
       </c>
       <c r="B61" t="n">
-        <v>609.0</v>
+        <v>14.0</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -1388,7 +1382,7 @@
         <v>62</v>
       </c>
       <c r="B62" t="n">
-        <v>677.0</v>
+        <v>36.0</v>
       </c>
       <c r="C62">
         <v>0</v>
@@ -1399,10 +1393,10 @@
         <v>63</v>
       </c>
       <c r="B63" t="n">
-        <v>575.0</v>
+        <v>8.0</v>
       </c>
       <c r="C63" t="n">
-        <v>43.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -1410,10 +1404,10 @@
         <v>64</v>
       </c>
       <c r="B64" t="n">
-        <v>427.0</v>
+        <v>3.0</v>
       </c>
       <c r="C64" t="n">
-        <v>56.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -1421,10 +1415,10 @@
         <v>65</v>
       </c>
       <c r="B65" t="n">
-        <v>294.0</v>
+        <v>0.0</v>
       </c>
       <c r="C65" t="n">
-        <v>83.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -1432,10 +1426,10 @@
         <v>66</v>
       </c>
       <c r="B66" t="n">
-        <v>228.0</v>
+        <v>0.0</v>
       </c>
       <c r="C66" t="n">
-        <v>71.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -1443,18 +1437,18 @@
         <v>67</v>
       </c>
       <c r="B67" t="n">
-        <v>223.0</v>
+        <v>0.0</v>
       </c>
       <c r="C67" t="n">
-        <v>81.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>68</v>
       </c>
-      <c r="B68" t="n">
-        <v>627.0</v>
+      <c r="B68">
+        <v>0</v>
       </c>
       <c r="C68">
         <v>0</v>
@@ -1464,8 +1458,8 @@
       <c r="A69" t="s">
         <v>69</v>
       </c>
-      <c r="B69" t="n">
-        <v>712.0</v>
+      <c r="B69">
+        <v>0</v>
       </c>
       <c r="C69">
         <v>0</v>
@@ -1475,8 +1469,8 @@
       <c r="A70" t="s">
         <v>70</v>
       </c>
-      <c r="B70" t="n">
-        <v>471.0</v>
+      <c r="B70">
+        <v>0</v>
       </c>
       <c r="C70">
         <v>0</v>
@@ -1486,8 +1480,8 @@
       <c r="A71" t="s">
         <v>71</v>
       </c>
-      <c r="B71" t="n">
-        <v>391.0</v>
+      <c r="B71">
+        <v>0</v>
       </c>
       <c r="C71">
         <v>0</v>
@@ -1497,8 +1491,8 @@
       <c r="A72" t="s">
         <v>72</v>
       </c>
-      <c r="B72" t="n">
-        <v>668.0</v>
+      <c r="B72">
+        <v>0</v>
       </c>
       <c r="C72">
         <v>0</v>
@@ -1508,8 +1502,8 @@
       <c r="A73" t="s">
         <v>73</v>
       </c>
-      <c r="B73" t="n">
-        <v>451.0</v>
+      <c r="B73">
+        <v>0</v>
       </c>
       <c r="C73">
         <v>0</v>
@@ -1519,55 +1513,55 @@
       <c r="A74" t="s">
         <v>74</v>
       </c>
-      <c r="B74" t="n">
-        <v>718.0</v>
-      </c>
-      <c r="C74" t="n">
-        <v>58.0</v>
+      <c r="B74">
+        <v>0</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>75</v>
       </c>
-      <c r="B75" t="n">
-        <v>477.0</v>
-      </c>
-      <c r="C75" t="n">
-        <v>61.0</v>
+      <c r="B75">
+        <v>0</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>76</v>
       </c>
-      <c r="B76" t="n">
-        <v>428.0</v>
-      </c>
-      <c r="C76" t="n">
-        <v>76.0</v>
+      <c r="B76">
+        <v>0</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>77</v>
       </c>
-      <c r="B77" t="n">
-        <v>435.0</v>
-      </c>
-      <c r="C77" t="n">
-        <v>64.0</v>
+      <c r="B77">
+        <v>0</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>78</v>
       </c>
-      <c r="B78" t="n">
-        <v>201.0</v>
-      </c>
-      <c r="C78" t="n">
-        <v>67.0</v>
+      <c r="B78">
+        <v>0</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -1575,7 +1569,7 @@
         <v>79</v>
       </c>
       <c r="B79" t="n">
-        <v>844.0</v>
+        <v>10.0</v>
       </c>
       <c r="C79">
         <v>0</v>
@@ -1586,7 +1580,7 @@
         <v>80</v>
       </c>
       <c r="B80" t="n">
-        <v>770.0</v>
+        <v>18.0</v>
       </c>
       <c r="C80">
         <v>0</v>
@@ -1597,7 +1591,7 @@
         <v>81</v>
       </c>
       <c r="B81" t="n">
-        <v>669.0</v>
+        <v>27.0</v>
       </c>
       <c r="C81">
         <v>0</v>
@@ -1608,7 +1602,7 @@
         <v>82</v>
       </c>
       <c r="B82" t="n">
-        <v>749.0</v>
+        <v>21.0</v>
       </c>
       <c r="C82">
         <v>0</v>
@@ -1619,7 +1613,7 @@
         <v>83</v>
       </c>
       <c r="B83" t="n">
-        <v>799.0</v>
+        <v>5.0</v>
       </c>
       <c r="C83">
         <v>0</v>
@@ -1630,7 +1624,7 @@
         <v>84</v>
       </c>
       <c r="B84" t="n">
-        <v>496.0</v>
+        <v>55.0</v>
       </c>
       <c r="C84">
         <v>0</v>
@@ -1641,10 +1635,10 @@
         <v>85</v>
       </c>
       <c r="B85" t="n">
-        <v>587.0</v>
+        <v>3.0</v>
       </c>
       <c r="C85" t="n">
-        <v>68.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -1652,10 +1646,10 @@
         <v>86</v>
       </c>
       <c r="B86" t="n">
-        <v>412.0</v>
+        <v>8.0</v>
       </c>
       <c r="C86" t="n">
-        <v>53.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -1663,10 +1657,10 @@
         <v>87</v>
       </c>
       <c r="B87" t="n">
-        <v>431.0</v>
+        <v>11.0</v>
       </c>
       <c r="C87" t="n">
-        <v>65.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -1674,21 +1668,21 @@
         <v>88</v>
       </c>
       <c r="B88" t="n">
-        <v>310.0</v>
+        <v>9.0</v>
       </c>
       <c r="C88" t="n">
-        <v>83.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B89" t="n">
-        <v>261.0</v>
+        <v>1.0</v>
       </c>
       <c r="C89" t="n">
-        <v>103.0</v>
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented overs in scorecard
</commit_message>
<xml_diff>
--- a/src/PlayerStanding/player_standings.xlsx
+++ b/src/PlayerStanding/player_standings.xlsx
@@ -721,8 +721,8 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
-        <v>0</v>
+      <c r="B2" t="n">
+        <v>6.0</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -732,8 +732,8 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
-        <v>0</v>
+      <c r="B3" t="n">
+        <v>11.0</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -743,8 +743,8 @@
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
-        <v>0</v>
+      <c r="B4" t="n">
+        <v>26.0</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -754,8 +754,8 @@
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5">
-        <v>0</v>
+      <c r="B5" t="n">
+        <v>3.0</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -765,8 +765,8 @@
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6">
-        <v>0</v>
+      <c r="B6" t="n">
+        <v>0.0</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -776,8 +776,8 @@
       <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B7">
-        <v>0</v>
+      <c r="B7" t="n">
+        <v>0.0</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -787,55 +787,55 @@
       <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
+      <c r="B8" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1.0</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
+      <c r="B9" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>2.0</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
+      <c r="B10" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>3.0</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
+      <c r="B11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>3.0</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
+      <c r="B12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1.0</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -963,8 +963,8 @@
       <c r="A24" t="s">
         <v>25</v>
       </c>
-      <c r="B24">
-        <v>0</v>
+      <c r="B24" t="n">
+        <v>20.0</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -974,8 +974,8 @@
       <c r="A25" t="s">
         <v>26</v>
       </c>
-      <c r="B25">
-        <v>0</v>
+      <c r="B25" t="n">
+        <v>56.0</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -985,8 +985,8 @@
       <c r="A26" t="s">
         <v>27</v>
       </c>
-      <c r="B26">
-        <v>0</v>
+      <c r="B26" t="n">
+        <v>23.0</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -996,8 +996,8 @@
       <c r="A27" t="s">
         <v>28</v>
       </c>
-      <c r="B27">
-        <v>0</v>
+      <c r="B27" t="n">
+        <v>50.0</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -1007,8 +1007,8 @@
       <c r="A28" t="s">
         <v>29</v>
       </c>
-      <c r="B28">
-        <v>0</v>
+      <c r="B28" t="n">
+        <v>0.0</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -1018,8 +1018,8 @@
       <c r="A29" t="s">
         <v>30</v>
       </c>
-      <c r="B29">
-        <v>0</v>
+      <c r="B29" t="n">
+        <v>0.0</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -1029,55 +1029,55 @@
       <c r="A30" t="s">
         <v>31</v>
       </c>
-      <c r="B30">
-        <v>0</v>
-      </c>
-      <c r="C30">
-        <v>0</v>
+      <c r="B30" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="C30" t="n">
+        <v>2.0</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>32</v>
       </c>
-      <c r="B31">
-        <v>0</v>
-      </c>
-      <c r="C31">
-        <v>0</v>
+      <c r="B31" t="n">
+        <v>43.0</v>
+      </c>
+      <c r="C31" t="n">
+        <v>6.0</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>33</v>
       </c>
-      <c r="B32">
-        <v>0</v>
-      </c>
-      <c r="C32">
-        <v>0</v>
+      <c r="B32" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="C32" t="n">
+        <v>3.0</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>34</v>
       </c>
-      <c r="B33">
-        <v>0</v>
-      </c>
-      <c r="C33">
-        <v>0</v>
+      <c r="B33" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="C33" t="n">
+        <v>4.0</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>35</v>
       </c>
-      <c r="B34">
-        <v>0</v>
-      </c>
-      <c r="C34">
-        <v>0</v>
+      <c r="B34" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C34" t="n">
+        <v>5.0</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1206,7 +1206,7 @@
         <v>46</v>
       </c>
       <c r="B46" t="n">
-        <v>22.0</v>
+        <v>28.0</v>
       </c>
       <c r="C46">
         <v>0</v>
@@ -1217,7 +1217,7 @@
         <v>47</v>
       </c>
       <c r="B47" t="n">
-        <v>56.0</v>
+        <v>78.0</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -1228,7 +1228,7 @@
         <v>48</v>
       </c>
       <c r="B48" t="n">
-        <v>75.0</v>
+        <v>110.0</v>
       </c>
       <c r="C48">
         <v>0</v>
@@ -1239,7 +1239,7 @@
         <v>49</v>
       </c>
       <c r="B49" t="n">
-        <v>49.0</v>
+        <v>83.0</v>
       </c>
       <c r="C49">
         <v>0</v>
@@ -1250,7 +1250,7 @@
         <v>50</v>
       </c>
       <c r="B50" t="n">
-        <v>54.0</v>
+        <v>134.0</v>
       </c>
       <c r="C50">
         <v>0</v>
@@ -1261,7 +1261,7 @@
         <v>51</v>
       </c>
       <c r="B51" t="n">
-        <v>19.0</v>
+        <v>28.0</v>
       </c>
       <c r="C51">
         <v>0</v>
@@ -1272,10 +1272,10 @@
         <v>52</v>
       </c>
       <c r="B52" t="n">
-        <v>45.0</v>
+        <v>51.0</v>
       </c>
       <c r="C52" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1283,10 +1283,10 @@
         <v>53</v>
       </c>
       <c r="B53" t="n">
-        <v>23.0</v>
+        <v>25.0</v>
       </c>
       <c r="C53" t="n">
-        <v>4.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -1294,10 +1294,10 @@
         <v>54</v>
       </c>
       <c r="B54" t="n">
+        <v>117.0</v>
+      </c>
+      <c r="C54" t="n">
         <v>9.0</v>
-      </c>
-      <c r="C54" t="n">
-        <v>3.0</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -1305,10 +1305,10 @@
         <v>55</v>
       </c>
       <c r="B55" t="n">
-        <v>33.0</v>
+        <v>49.0</v>
       </c>
       <c r="C55" t="n">
-        <v>5.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -1316,10 +1316,10 @@
         <v>56</v>
       </c>
       <c r="B56" t="n">
-        <v>6.0</v>
+        <v>21.0</v>
       </c>
       <c r="C56" t="n">
-        <v>6.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -1327,7 +1327,7 @@
         <v>57</v>
       </c>
       <c r="B57" t="n">
-        <v>68.0</v>
+        <v>83.0</v>
       </c>
       <c r="C57">
         <v>0</v>
@@ -1349,7 +1349,7 @@
         <v>59</v>
       </c>
       <c r="B59" t="n">
-        <v>20.0</v>
+        <v>46.0</v>
       </c>
       <c r="C59">
         <v>0</v>
@@ -1360,7 +1360,7 @@
         <v>60</v>
       </c>
       <c r="B60" t="n">
-        <v>72.0</v>
+        <v>117.0</v>
       </c>
       <c r="C60">
         <v>0</v>
@@ -1371,7 +1371,7 @@
         <v>61</v>
       </c>
       <c r="B61" t="n">
-        <v>166.0</v>
+        <v>227.0</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -1382,7 +1382,7 @@
         <v>62</v>
       </c>
       <c r="B62" t="n">
-        <v>54.0</v>
+        <v>59.0</v>
       </c>
       <c r="C62">
         <v>0</v>
@@ -1393,10 +1393,10 @@
         <v>63</v>
       </c>
       <c r="B63" t="n">
-        <v>18.0</v>
+        <v>30.0</v>
       </c>
       <c r="C63" t="n">
-        <v>8.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -1404,10 +1404,10 @@
         <v>64</v>
       </c>
       <c r="B64" t="n">
-        <v>24.0</v>
+        <v>34.0</v>
       </c>
       <c r="C64" t="n">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -1415,10 +1415,10 @@
         <v>65</v>
       </c>
       <c r="B65" t="n">
-        <v>13.0</v>
+        <v>19.0</v>
       </c>
       <c r="C65" t="n">
-        <v>5.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -1426,10 +1426,10 @@
         <v>66</v>
       </c>
       <c r="B66" t="n">
-        <v>20.0</v>
+        <v>28.0</v>
       </c>
       <c r="C66" t="n">
-        <v>5.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -1437,10 +1437,10 @@
         <v>67</v>
       </c>
       <c r="B67" t="n">
-        <v>53.0</v>
+        <v>64.0</v>
       </c>
       <c r="C67" t="n">
-        <v>7.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -1448,7 +1448,7 @@
         <v>68</v>
       </c>
       <c r="B68" t="n">
-        <v>9.0</v>
+        <v>21.0</v>
       </c>
       <c r="C68">
         <v>0</v>
@@ -1459,7 +1459,7 @@
         <v>69</v>
       </c>
       <c r="B69" t="n">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
       <c r="C69">
         <v>0</v>
@@ -1470,7 +1470,7 @@
         <v>70</v>
       </c>
       <c r="B70" t="n">
-        <v>21.0</v>
+        <v>38.0</v>
       </c>
       <c r="C70">
         <v>0</v>
@@ -1481,7 +1481,7 @@
         <v>71</v>
       </c>
       <c r="B71" t="n">
-        <v>4.0</v>
+        <v>65.0</v>
       </c>
       <c r="C71">
         <v>0</v>
@@ -1492,7 +1492,7 @@
         <v>72</v>
       </c>
       <c r="B72" t="n">
-        <v>13.0</v>
+        <v>65.0</v>
       </c>
       <c r="C72">
         <v>0</v>
@@ -1503,7 +1503,7 @@
         <v>73</v>
       </c>
       <c r="B73" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="C73">
         <v>0</v>
@@ -1514,10 +1514,10 @@
         <v>74</v>
       </c>
       <c r="B74" t="n">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
       <c r="C74" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -1528,7 +1528,7 @@
         <v>57.0</v>
       </c>
       <c r="C75" t="n">
-        <v>3.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -1536,10 +1536,10 @@
         <v>76</v>
       </c>
       <c r="B76" t="n">
-        <v>42.0</v>
+        <v>80.0</v>
       </c>
       <c r="C76" t="n">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -1547,7 +1547,7 @@
         <v>77</v>
       </c>
       <c r="B77" t="n">
-        <v>60.0</v>
+        <v>88.0</v>
       </c>
       <c r="C77" t="n">
         <v>1.0</v>
@@ -1558,10 +1558,10 @@
         <v>78</v>
       </c>
       <c r="B78" t="n">
-        <v>22.0</v>
+        <v>34.0</v>
       </c>
       <c r="C78" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -1569,7 +1569,7 @@
         <v>79</v>
       </c>
       <c r="B79" t="n">
-        <v>10.0</v>
+        <v>15.0</v>
       </c>
       <c r="C79">
         <v>0</v>
@@ -1580,7 +1580,7 @@
         <v>80</v>
       </c>
       <c r="B80" t="n">
-        <v>18.0</v>
+        <v>29.0</v>
       </c>
       <c r="C80">
         <v>0</v>
@@ -1591,7 +1591,7 @@
         <v>81</v>
       </c>
       <c r="B81" t="n">
-        <v>27.0</v>
+        <v>58.0</v>
       </c>
       <c r="C81">
         <v>0</v>
@@ -1602,7 +1602,7 @@
         <v>82</v>
       </c>
       <c r="B82" t="n">
-        <v>21.0</v>
+        <v>54.0</v>
       </c>
       <c r="C82">
         <v>0</v>
@@ -1613,7 +1613,7 @@
         <v>83</v>
       </c>
       <c r="B83" t="n">
-        <v>5.0</v>
+        <v>46.0</v>
       </c>
       <c r="C83">
         <v>0</v>
@@ -1624,7 +1624,7 @@
         <v>84</v>
       </c>
       <c r="B84" t="n">
-        <v>55.0</v>
+        <v>71.0</v>
       </c>
       <c r="C84">
         <v>0</v>
@@ -1635,10 +1635,10 @@
         <v>85</v>
       </c>
       <c r="B85" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="C85" t="n">
         <v>3.0</v>
-      </c>
-      <c r="C85" t="n">
-        <v>2.0</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -1646,10 +1646,10 @@
         <v>86</v>
       </c>
       <c r="B86" t="n">
-        <v>8.0</v>
+        <v>39.0</v>
       </c>
       <c r="C86" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -1657,10 +1657,10 @@
         <v>87</v>
       </c>
       <c r="B87" t="n">
-        <v>11.0</v>
+        <v>35.0</v>
       </c>
       <c r="C87" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -1668,10 +1668,10 @@
         <v>88</v>
       </c>
       <c r="B88" t="n">
-        <v>9.0</v>
+        <v>24.0</v>
       </c>
       <c r="C88" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -1679,10 +1679,10 @@
         <v>90</v>
       </c>
       <c r="B89" t="n">
-        <v>1.0</v>
+        <v>12.0</v>
       </c>
       <c r="C89" t="n">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new color to start match
</commit_message>
<xml_diff>
--- a/src/PlayerStanding/player_standings.xlsx
+++ b/src/PlayerStanding/player_standings.xlsx
@@ -733,7 +733,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="n">
-        <v>28.0</v>
+        <v>29.0</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -744,7 +744,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="n">
-        <v>42.0</v>
+        <v>80.0</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -755,7 +755,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="n">
-        <v>3.0</v>
+        <v>8.0</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -791,7 +791,7 @@
         <v>11.0</v>
       </c>
       <c r="C8" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -799,7 +799,7 @@
         <v>10</v>
       </c>
       <c r="B9" t="n">
-        <v>21.0</v>
+        <v>33.0</v>
       </c>
       <c r="C9" t="n">
         <v>2.0</v>
@@ -810,10 +810,10 @@
         <v>11</v>
       </c>
       <c r="B10" t="n">
-        <v>29.0</v>
+        <v>35.0</v>
       </c>
       <c r="C10" t="n">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -821,7 +821,7 @@
         <v>12</v>
       </c>
       <c r="B11" t="n">
-        <v>12.0</v>
+        <v>28.0</v>
       </c>
       <c r="C11" t="n">
         <v>4.0</v>
@@ -832,10 +832,10 @@
         <v>13</v>
       </c>
       <c r="B12" t="n">
-        <v>0.0</v>
+        <v>24.0</v>
       </c>
       <c r="C12" t="n">
-        <v>3.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1206,7 +1206,7 @@
         <v>46</v>
       </c>
       <c r="B46" t="n">
-        <v>90.0</v>
+        <v>96.0</v>
       </c>
       <c r="C46">
         <v>0</v>
@@ -1217,7 +1217,7 @@
         <v>47</v>
       </c>
       <c r="B47" t="n">
-        <v>90.0</v>
+        <v>100.0</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -1228,7 +1228,7 @@
         <v>48</v>
       </c>
       <c r="B48" t="n">
-        <v>214.0</v>
+        <v>238.0</v>
       </c>
       <c r="C48">
         <v>0</v>
@@ -1239,7 +1239,7 @@
         <v>49</v>
       </c>
       <c r="B49" t="n">
-        <v>178.0</v>
+        <v>183.0</v>
       </c>
       <c r="C49">
         <v>0</v>
@@ -1250,7 +1250,7 @@
         <v>50</v>
       </c>
       <c r="B50" t="n">
-        <v>155.0</v>
+        <v>157.0</v>
       </c>
       <c r="C50">
         <v>0</v>
@@ -1261,7 +1261,7 @@
         <v>51</v>
       </c>
       <c r="B51" t="n">
-        <v>52.0</v>
+        <v>60.0</v>
       </c>
       <c r="C51">
         <v>0</v>
@@ -1272,7 +1272,7 @@
         <v>52</v>
       </c>
       <c r="B52" t="n">
-        <v>95.0</v>
+        <v>102.0</v>
       </c>
       <c r="C52" t="n">
         <v>9.0</v>
@@ -1283,7 +1283,7 @@
         <v>53</v>
       </c>
       <c r="B53" t="n">
-        <v>42.0</v>
+        <v>46.0</v>
       </c>
       <c r="C53" t="n">
         <v>18.0</v>
@@ -1294,7 +1294,7 @@
         <v>54</v>
       </c>
       <c r="B54" t="n">
-        <v>134.0</v>
+        <v>146.0</v>
       </c>
       <c r="C54" t="n">
         <v>12.0</v>
@@ -1308,7 +1308,7 @@
         <v>77.0</v>
       </c>
       <c r="C55" t="n">
-        <v>12.0</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -1316,10 +1316,10 @@
         <v>56</v>
       </c>
       <c r="B56" t="n">
-        <v>41.0</v>
+        <v>48.0</v>
       </c>
       <c r="C56" t="n">
-        <v>17.0</v>
+        <v>22.0</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -1371,7 +1371,7 @@
         <v>61</v>
       </c>
       <c r="B61" t="n">
-        <v>227.0</v>
+        <v>263.0</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -1382,7 +1382,7 @@
         <v>62</v>
       </c>
       <c r="B62" t="n">
-        <v>59.0</v>
+        <v>99.0</v>
       </c>
       <c r="C62">
         <v>0</v>
@@ -1396,7 +1396,7 @@
         <v>30.0</v>
       </c>
       <c r="C63" t="n">
-        <v>10.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -1407,7 +1407,7 @@
         <v>34.0</v>
       </c>
       <c r="C64" t="n">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -1415,10 +1415,10 @@
         <v>65</v>
       </c>
       <c r="B65" t="n">
-        <v>19.0</v>
+        <v>24.0</v>
       </c>
       <c r="C65" t="n">
-        <v>7.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -1426,10 +1426,10 @@
         <v>66</v>
       </c>
       <c r="B66" t="n">
-        <v>28.0</v>
+        <v>33.0</v>
       </c>
       <c r="C66" t="n">
-        <v>7.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -1440,7 +1440,7 @@
         <v>64.0</v>
       </c>
       <c r="C67" t="n">
-        <v>10.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -1470,7 +1470,7 @@
         <v>70</v>
       </c>
       <c r="B70" t="n">
-        <v>45.0</v>
+        <v>92.0</v>
       </c>
       <c r="C70">
         <v>0</v>
@@ -1481,7 +1481,7 @@
         <v>71</v>
       </c>
       <c r="B71" t="n">
-        <v>71.0</v>
+        <v>95.0</v>
       </c>
       <c r="C71">
         <v>0</v>
@@ -1492,7 +1492,7 @@
         <v>72</v>
       </c>
       <c r="B72" t="n">
-        <v>65.0</v>
+        <v>83.0</v>
       </c>
       <c r="C72">
         <v>0</v>
@@ -1503,7 +1503,7 @@
         <v>73</v>
       </c>
       <c r="B73" t="n">
-        <v>22.0</v>
+        <v>28.0</v>
       </c>
       <c r="C73">
         <v>0</v>
@@ -1517,7 +1517,7 @@
         <v>10.0</v>
       </c>
       <c r="C74" t="n">
-        <v>6.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -1525,10 +1525,10 @@
         <v>75</v>
       </c>
       <c r="B75" t="n">
-        <v>103.0</v>
+        <v>115.0</v>
       </c>
       <c r="C75" t="n">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -1539,7 +1539,7 @@
         <v>94.0</v>
       </c>
       <c r="C76" t="n">
-        <v>6.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -1550,7 +1550,7 @@
         <v>110.0</v>
       </c>
       <c r="C77" t="n">
-        <v>5.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -1561,7 +1561,7 @@
         <v>46.0</v>
       </c>
       <c r="C78" t="n">
-        <v>6.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>